<commit_message>
Enquiry & Daily Status Tracker
Enquiry & Daily Status Tracker
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/DailyStatusTracker.xlsx
+++ b/Offline/BusinessManagement/DailyStatusTracker.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E5550B7-D93C-470F-9A4C-D75F240030F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E3DA68B-2A49-4745-81E5-A0D8A330E947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tracker" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="127">
   <si>
     <t>Item Number</t>
   </si>
@@ -391,6 +391,18 @@
   </si>
   <si>
     <t>To start in Feb 4th week</t>
+  </si>
+  <si>
+    <t>Off Day</t>
+  </si>
+  <si>
+    <t>Out Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In Time </t>
+  </si>
+  <si>
+    <t>Day</t>
   </si>
 </sst>
 </file>
@@ -475,7 +487,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -498,6 +510,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -805,24 +821,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G19" sqref="G19"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.33203125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="39.19921875" customWidth="1"/>
-    <col min="3" max="3" width="14.53125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.21875" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="78.3984375" customWidth="1"/>
-    <col min="8" max="8" width="15.796875" customWidth="1"/>
+    <col min="7" max="7" width="78.44140625" customWidth="1"/>
+    <col min="8" max="8" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -848,7 +864,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="11">
         <v>1</v>
       </c>
@@ -869,7 +885,7 @@
       </c>
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="11">
         <v>2</v>
       </c>
@@ -890,7 +906,7 @@
       </c>
       <c r="G3" s="10"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="11">
         <v>3</v>
       </c>
@@ -911,7 +927,7 @@
       </c>
       <c r="G4" s="10"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="11">
         <v>4</v>
       </c>
@@ -934,7 +950,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="11">
         <v>5</v>
       </c>
@@ -957,7 +973,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="11">
         <v>6</v>
       </c>
@@ -980,7 +996,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="11">
         <v>7</v>
       </c>
@@ -1003,7 +1019,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="11">
         <v>8</v>
       </c>
@@ -1026,7 +1042,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="11">
         <v>9</v>
       </c>
@@ -1049,7 +1065,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="11">
         <v>10</v>
       </c>
@@ -1072,7 +1088,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="11">
         <v>11</v>
       </c>
@@ -1095,7 +1111,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="11">
         <v>12</v>
       </c>
@@ -1118,7 +1134,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="11">
         <v>13</v>
       </c>
@@ -1141,7 +1157,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="11">
         <v>14</v>
       </c>
@@ -1164,7 +1180,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="11">
         <v>15</v>
       </c>
@@ -1187,7 +1203,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="11">
         <v>16</v>
       </c>
@@ -1208,7 +1224,7 @@
       </c>
       <c r="G17" s="10"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="11">
         <v>17</v>
       </c>
@@ -1231,7 +1247,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -1264,13 +1280,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F24168E-DBD7-4361-AEEA-D57845BDFBC0}">
   <dimension ref="A2:F54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="145.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>23</v>
       </c>
@@ -1290,7 +1309,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>24</v>
       </c>
@@ -1310,7 +1329,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>25</v>
       </c>
@@ -1330,7 +1349,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>26</v>
       </c>
@@ -1350,7 +1369,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>20</v>
       </c>
@@ -1370,7 +1389,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>21</v>
       </c>
@@ -1390,7 +1409,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>28</v>
       </c>
@@ -1401,7 +1420,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>29</v>
       </c>
@@ -1412,7 +1431,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>30</v>
       </c>
@@ -1423,7 +1442,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>31</v>
       </c>
@@ -1434,7 +1453,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>32</v>
       </c>
@@ -1445,7 +1464,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>33</v>
       </c>
@@ -1456,7 +1475,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>34</v>
       </c>
@@ -1467,7 +1486,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>35</v>
       </c>
@@ -1478,7 +1497,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>36</v>
       </c>
@@ -1489,7 +1508,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>37</v>
       </c>
@@ -1500,7 +1519,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>38</v>
       </c>
@@ -1511,7 +1530,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="57" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>39</v>
       </c>
@@ -1522,7 +1541,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>40</v>
       </c>
@@ -1533,7 +1552,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>41</v>
       </c>
@@ -1544,7 +1563,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <v>42</v>
       </c>
@@ -1555,7 +1574,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>43</v>
       </c>
@@ -1566,7 +1585,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
         <v>44</v>
       </c>
@@ -1577,7 +1596,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
         <v>45</v>
       </c>
@@ -1588,7 +1607,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
         <v>46</v>
       </c>
@@ -1599,7 +1618,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
         <v>47</v>
       </c>
@@ -1610,7 +1629,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="5">
         <v>48</v>
       </c>
@@ -1621,7 +1640,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="5">
         <v>49</v>
       </c>
@@ -1632,7 +1651,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
         <v>50</v>
       </c>
@@ -1643,7 +1662,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="5">
         <v>51</v>
       </c>
@@ -1654,7 +1673,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="5">
         <v>52</v>
       </c>
@@ -1665,7 +1684,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="5">
         <v>53</v>
       </c>
@@ -1676,7 +1695,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="5">
         <v>54</v>
       </c>
@@ -1687,7 +1706,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="5">
         <v>55</v>
       </c>
@@ -1698,7 +1717,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="5">
         <v>56</v>
       </c>
@@ -1709,7 +1728,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="5">
         <v>57</v>
       </c>
@@ -1720,7 +1739,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="5">
         <v>58</v>
       </c>
@@ -1731,7 +1750,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="5">
         <v>59</v>
       </c>
@@ -1742,7 +1761,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="5">
         <v>60</v>
       </c>
@@ -1753,7 +1772,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="5">
         <v>61</v>
       </c>
@@ -1764,7 +1783,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="5">
         <v>62</v>
       </c>
@@ -1775,7 +1794,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="5">
         <v>63</v>
       </c>
@@ -1786,7 +1805,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="5">
         <v>64</v>
       </c>
@@ -1797,7 +1816,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="5">
         <v>65</v>
       </c>
@@ -1808,7 +1827,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="5">
         <v>66</v>
       </c>
@@ -1819,7 +1838,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="5">
         <v>67</v>
       </c>
@@ -1830,7 +1849,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="5">
         <v>69</v>
       </c>
@@ -1841,7 +1860,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="5">
         <v>70</v>
       </c>
@@ -1852,7 +1871,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="5">
         <v>71</v>
       </c>
@@ -1863,7 +1882,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="5">
         <v>72</v>
       </c>
@@ -1874,7 +1893,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="5">
         <v>73</v>
       </c>
@@ -1885,7 +1904,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="5">
         <v>74</v>
       </c>
@@ -1896,7 +1915,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="5">
         <v>75</v>
       </c>
@@ -1914,24 +1933,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B2:I7"/>
+  <dimension ref="B2:N9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="7.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.3984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.86328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>17</v>
       </c>
@@ -1956,8 +1976,17 @@
       <c r="I2" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="L2" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B3" s="8" t="s">
         <v>31</v>
       </c>
@@ -1982,8 +2011,17 @@
       <c r="I3" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="L3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" s="13">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="N3" s="13">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B4" s="9" t="s">
         <v>18</v>
       </c>
@@ -2008,8 +2046,17 @@
       <c r="I4" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="L4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M4" s="13">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="N4" s="13">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B5" s="8" t="s">
         <v>19</v>
       </c>
@@ -2034,8 +2081,15 @@
       <c r="I5" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="L5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="M5" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="N5" s="14"/>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B6" s="9" t="s">
         <v>21</v>
       </c>
@@ -2060,8 +2114,17 @@
       <c r="I6" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="L6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M6" s="13">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="N6" s="13">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B7" s="9" t="s">
         <v>20</v>
       </c>
@@ -2086,8 +2149,42 @@
       <c r="I7" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="L7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="M7" s="13">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="N7" s="13">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="L8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M8" s="13">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="N8" s="13">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="L9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M9" s="13">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="N9" s="13">
+        <v>0.75</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="M5:N5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated daily status tracker
Updated daily status tracker
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/DailyStatusTracker.xlsx
+++ b/Offline/BusinessManagement/DailyStatusTracker.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF8F33DE-A7D6-402D-8CB9-6109AF35A5B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70DE83C7-75C3-4C35-9F30-A062C60561BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tracker" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="WorkDays" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tracker!$A$1:$H$18</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tracker!$A$1:$H$20</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
 </workbook>
@@ -816,23 +816,23 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.33203125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="41.53125" customWidth="1"/>
-    <col min="3" max="3" width="14.53125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.5546875" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.6640625" customWidth="1"/>
-    <col min="5" max="5" width="9.1328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="93.796875" customWidth="1"/>
-    <col min="8" max="8" width="15.796875" customWidth="1"/>
+    <col min="7" max="7" width="93.77734375" customWidth="1"/>
+    <col min="8" max="8" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -858,7 +858,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="11">
         <v>1</v>
       </c>
@@ -879,7 +879,7 @@
       </c>
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="11">
         <v>2</v>
       </c>
@@ -900,7 +900,7 @@
       </c>
       <c r="G3" s="10"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="11">
         <v>3</v>
       </c>
@@ -921,7 +921,7 @@
       </c>
       <c r="G4" s="10"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="11">
         <v>4</v>
       </c>
@@ -942,7 +942,7 @@
       </c>
       <c r="G5" s="10"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="11">
         <v>5</v>
       </c>
@@ -963,7 +963,7 @@
       </c>
       <c r="G6" s="10"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="11">
         <v>6</v>
       </c>
@@ -984,7 +984,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="11">
         <v>7</v>
       </c>
@@ -1007,7 +1007,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="11">
         <v>8</v>
       </c>
@@ -1030,7 +1030,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="11">
         <v>9</v>
       </c>
@@ -1053,7 +1053,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="228" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A11" s="11">
         <v>10</v>
       </c>
@@ -1076,7 +1076,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="11">
         <v>11</v>
       </c>
@@ -1099,7 +1099,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="11">
         <v>12</v>
       </c>
@@ -1122,7 +1122,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="11">
         <v>13</v>
       </c>
@@ -1145,7 +1145,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="11">
         <v>14</v>
       </c>
@@ -1168,7 +1168,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="11">
         <v>15</v>
       </c>
@@ -1191,9 +1191,9 @@
         <v>93</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="11">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>12</v>
@@ -1214,9 +1214,9 @@
         <v>114</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="11">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>111</v>
@@ -1237,9 +1237,9 @@
         <v>115</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="11">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="10" t="s">
         <v>122</v>
@@ -1260,9 +1260,9 @@
         <v>118</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="11">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" s="10" t="s">
         <v>121</v>
@@ -1284,7 +1284,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H18" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:H20" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1297,9 +1297,9 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>23</v>
       </c>
@@ -1319,7 +1319,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>24</v>
       </c>
@@ -1339,7 +1339,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>25</v>
       </c>
@@ -1359,7 +1359,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>26</v>
       </c>
@@ -1379,7 +1379,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>20</v>
       </c>
@@ -1399,7 +1399,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>21</v>
       </c>
@@ -1419,7 +1419,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>28</v>
       </c>
@@ -1430,7 +1430,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>29</v>
       </c>
@@ -1441,7 +1441,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>30</v>
       </c>
@@ -1452,7 +1452,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>31</v>
       </c>
@@ -1463,7 +1463,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>32</v>
       </c>
@@ -1474,7 +1474,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>33</v>
       </c>
@@ -1485,7 +1485,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>34</v>
       </c>
@@ -1496,7 +1496,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>35</v>
       </c>
@@ -1507,7 +1507,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>36</v>
       </c>
@@ -1518,7 +1518,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>37</v>
       </c>
@@ -1529,7 +1529,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>38</v>
       </c>
@@ -1540,7 +1540,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="57" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>39</v>
       </c>
@@ -1551,7 +1551,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>40</v>
       </c>
@@ -1562,7 +1562,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>41</v>
       </c>
@@ -1573,7 +1573,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <v>42</v>
       </c>
@@ -1584,7 +1584,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>43</v>
       </c>
@@ -1595,7 +1595,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
         <v>44</v>
       </c>
@@ -1606,7 +1606,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
         <v>45</v>
       </c>
@@ -1617,7 +1617,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
         <v>46</v>
       </c>
@@ -1628,7 +1628,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
         <v>47</v>
       </c>
@@ -1639,7 +1639,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="5">
         <v>48</v>
       </c>
@@ -1650,7 +1650,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="5">
         <v>49</v>
       </c>
@@ -1661,7 +1661,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
         <v>50</v>
       </c>
@@ -1672,7 +1672,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="5">
         <v>51</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="5">
         <v>52</v>
       </c>
@@ -1694,7 +1694,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="5">
         <v>53</v>
       </c>
@@ -1705,7 +1705,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="5">
         <v>54</v>
       </c>
@@ -1716,7 +1716,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="5">
         <v>55</v>
       </c>
@@ -1727,7 +1727,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="5">
         <v>56</v>
       </c>
@@ -1738,7 +1738,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="5">
         <v>57</v>
       </c>
@@ -1749,7 +1749,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="5">
         <v>58</v>
       </c>
@@ -1760,7 +1760,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="5">
         <v>59</v>
       </c>
@@ -1771,7 +1771,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="5">
         <v>60</v>
       </c>
@@ -1782,7 +1782,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="5">
         <v>61</v>
       </c>
@@ -1793,7 +1793,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="5">
         <v>62</v>
       </c>
@@ -1804,7 +1804,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="5">
         <v>63</v>
       </c>
@@ -1815,7 +1815,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="5">
         <v>64</v>
       </c>
@@ -1826,7 +1826,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="5">
         <v>65</v>
       </c>
@@ -1837,7 +1837,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="5">
         <v>66</v>
       </c>
@@ -1848,7 +1848,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="5">
         <v>67</v>
       </c>
@@ -1859,7 +1859,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="5">
         <v>69</v>
       </c>
@@ -1870,7 +1870,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="5">
         <v>70</v>
       </c>
@@ -1881,7 +1881,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="5">
         <v>71</v>
       </c>
@@ -1892,7 +1892,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="5">
         <v>72</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="5">
         <v>73</v>
       </c>
@@ -1914,7 +1914,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="5">
         <v>74</v>
       </c>
@@ -1925,7 +1925,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="5">
         <v>75</v>
       </c>
@@ -1949,18 +1949,18 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="7.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.3984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.86328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>16</v>
       </c>
@@ -1986,7 +1986,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B3" s="8" t="s">
         <v>30</v>
       </c>
@@ -2012,7 +2012,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B4" s="9" t="s">
         <v>17</v>
       </c>
@@ -2038,7 +2038,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5" s="8" t="s">
         <v>18</v>
       </c>
@@ -2064,7 +2064,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" s="9" t="s">
         <v>20</v>
       </c>
@@ -2090,7 +2090,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7" s="9" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
Update Daily Status Track
Update Daily Status Track
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/DailyStatusTracker.xlsx
+++ b/Offline/BusinessManagement/DailyStatusTracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70DE83C7-75C3-4C35-9F30-A062C60561BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{788449B1-74FF-41A1-AE5A-ADBDF51240AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -816,14 +816,14 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.33203125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="41.5546875" customWidth="1"/>
+    <col min="2" max="2" width="50" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.6640625" customWidth="1"/>
     <col min="5" max="5" width="9.109375" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
Daily Status Track updated
Daily Status Track updated
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/DailyStatusTracker.xlsx
+++ b/Offline/BusinessManagement/DailyStatusTracker.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCB6009F-41B0-42AF-9315-D0463EBA5B67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6497D05-78E6-42AB-980C-96C5E98EC84B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tracker" sheetId="1" r:id="rId1"/>
@@ -13,14 +13,14 @@
     <sheet name="WorkDays" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tracker!$A$1:$H$25</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tracker!$A$1:$H$29</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="137">
   <si>
     <t>Item Number</t>
   </si>
@@ -444,6 +444,9 @@
     B. Use onclick event of same button to open anodiam app if it is already installed
 4. Test the responsiveness of https://www.google.business.sample.site
 5. Must have a button "Visit anodiam.com website": upon clicking it will open anodiam.com &gt;&gt; classplus/YOWWA website</t>
+  </si>
+  <si>
+    <t>Sent mail to class plus. Waiting for reply.</t>
   </si>
 </sst>
 </file>
@@ -868,23 +871,23 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.33203125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="50" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.53125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="72" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.6640625" customWidth="1"/>
-    <col min="5" max="5" width="9.1328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="93.796875" customWidth="1"/>
-    <col min="8" max="8" width="15.796875" customWidth="1"/>
+    <col min="7" max="7" width="93.77734375" customWidth="1"/>
+    <col min="8" max="8" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -910,7 +913,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="11">
         <v>1</v>
       </c>
@@ -931,7 +934,7 @@
       </c>
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="11">
         <v>2</v>
       </c>
@@ -952,7 +955,7 @@
       </c>
       <c r="G3" s="10"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="11">
         <v>3</v>
       </c>
@@ -973,7 +976,7 @@
       </c>
       <c r="G4" s="10"/>
     </row>
-    <row r="5" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="12">
         <v>4</v>
       </c>
@@ -994,7 +997,7 @@
       </c>
       <c r="G5" s="13"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="11">
         <v>5</v>
       </c>
@@ -1017,7 +1020,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="11">
         <v>6</v>
       </c>
@@ -1038,7 +1041,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="12">
         <v>7</v>
       </c>
@@ -1059,7 +1062,7 @@
       </c>
       <c r="G8" s="13"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="11">
         <v>8</v>
       </c>
@@ -1082,7 +1085,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="11">
         <v>9</v>
       </c>
@@ -1105,7 +1108,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="11">
         <v>10</v>
       </c>
@@ -1128,7 +1131,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="11">
         <v>11</v>
       </c>
@@ -1151,7 +1154,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="11">
         <v>12</v>
       </c>
@@ -1174,7 +1177,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="256.5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A14" s="11">
         <v>13</v>
       </c>
@@ -1197,7 +1200,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="12">
         <v>14</v>
       </c>
@@ -1220,7 +1223,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="12">
         <v>15</v>
       </c>
@@ -1244,7 +1247,7 @@
       </c>
       <c r="H16" s="14"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="11">
         <v>16</v>
       </c>
@@ -1267,7 +1270,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="11">
         <v>17</v>
       </c>
@@ -1290,7 +1293,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="11">
         <v>18</v>
       </c>
@@ -1313,7 +1316,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="11">
         <v>19</v>
       </c>
@@ -1336,7 +1339,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="11">
         <v>20</v>
       </c>
@@ -1359,7 +1362,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="11">
         <v>21</v>
       </c>
@@ -1382,7 +1385,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="11">
         <v>22</v>
       </c>
@@ -1405,7 +1408,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="11">
         <v>23</v>
       </c>
@@ -1425,27 +1428,27 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A25" s="11">
+    <row r="25" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="12">
         <v>25</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="D25" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="E25" s="10">
-        <v>5</v>
-      </c>
-      <c r="F25" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="E25" s="13">
+        <v>5</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
         <v>26</v>
       </c>
@@ -1465,7 +1468,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
         <v>27</v>
       </c>
@@ -1482,10 +1485,13 @@
         <v>5</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="5">
         <v>28</v>
       </c>
@@ -1502,10 +1508,13 @@
         <v>5</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="5">
         <v>29</v>
       </c>
@@ -1522,11 +1531,19 @@
         <v>5</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H25" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:H29" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1048576" xr:uid="{F694DCE3-45FE-4850-A54A-8379FCD46E21}">
+      <formula1>"Todo,WIP,Done"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1539,9 +1556,9 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>23</v>
       </c>
@@ -1561,7 +1578,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>24</v>
       </c>
@@ -1581,7 +1598,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>25</v>
       </c>
@@ -1601,7 +1618,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>26</v>
       </c>
@@ -1621,7 +1638,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>20</v>
       </c>
@@ -1641,7 +1658,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>21</v>
       </c>
@@ -1661,7 +1678,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>28</v>
       </c>
@@ -1672,7 +1689,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>29</v>
       </c>
@@ -1683,7 +1700,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>30</v>
       </c>
@@ -1694,7 +1711,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>31</v>
       </c>
@@ -1705,7 +1722,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>32</v>
       </c>
@@ -1716,7 +1733,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>33</v>
       </c>
@@ -1727,7 +1744,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>34</v>
       </c>
@@ -1738,7 +1755,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>35</v>
       </c>
@@ -1749,7 +1766,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>36</v>
       </c>
@@ -1760,7 +1777,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>37</v>
       </c>
@@ -1771,7 +1788,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>38</v>
       </c>
@@ -1782,7 +1799,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="409.5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>39</v>
       </c>
@@ -1793,7 +1810,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>40</v>
       </c>
@@ -1804,7 +1821,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>41</v>
       </c>
@@ -1815,7 +1832,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <v>42</v>
       </c>
@@ -1826,7 +1843,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>43</v>
       </c>
@@ -1837,7 +1854,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
         <v>44</v>
       </c>
@@ -1848,7 +1865,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
         <v>45</v>
       </c>
@@ -1859,7 +1876,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
         <v>46</v>
       </c>
@@ -1870,7 +1887,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
         <v>47</v>
       </c>
@@ -1881,7 +1898,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="5">
         <v>48</v>
       </c>
@@ -1892,7 +1909,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="5">
         <v>49</v>
       </c>
@@ -1903,7 +1920,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
         <v>50</v>
       </c>
@@ -1914,7 +1931,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="5">
         <v>51</v>
       </c>
@@ -1925,7 +1942,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="5">
         <v>52</v>
       </c>
@@ -1936,7 +1953,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="5">
         <v>53</v>
       </c>
@@ -1947,7 +1964,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="5">
         <v>54</v>
       </c>
@@ -1958,7 +1975,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="5">
         <v>55</v>
       </c>
@@ -1969,7 +1986,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="5">
         <v>56</v>
       </c>
@@ -1980,7 +1997,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="5">
         <v>57</v>
       </c>
@@ -1991,7 +2008,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="5">
         <v>58</v>
       </c>
@@ -2002,7 +2019,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="5">
         <v>59</v>
       </c>
@@ -2013,7 +2030,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="5">
         <v>60</v>
       </c>
@@ -2024,7 +2041,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="5">
         <v>61</v>
       </c>
@@ -2035,7 +2052,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="5">
         <v>62</v>
       </c>
@@ -2046,7 +2063,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="5">
         <v>63</v>
       </c>
@@ -2057,7 +2074,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="5">
         <v>64</v>
       </c>
@@ -2068,7 +2085,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="5">
         <v>65</v>
       </c>
@@ -2079,7 +2096,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="5">
         <v>66</v>
       </c>
@@ -2090,7 +2107,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="5">
         <v>67</v>
       </c>
@@ -2101,7 +2118,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="5">
         <v>69</v>
       </c>
@@ -2112,7 +2129,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="5">
         <v>70</v>
       </c>
@@ -2123,7 +2140,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="5">
         <v>71</v>
       </c>
@@ -2134,7 +2151,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="5">
         <v>72</v>
       </c>
@@ -2145,7 +2162,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="5">
         <v>73</v>
       </c>
@@ -2156,7 +2173,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="5">
         <v>74</v>
       </c>
@@ -2167,7 +2184,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="5">
         <v>75</v>
       </c>
@@ -2191,18 +2208,18 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.19921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="7.46484375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.19921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.19921875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.46484375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.86328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.46484375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>16</v>
       </c>
@@ -2228,7 +2245,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B3" s="8" t="s">
         <v>30</v>
       </c>
@@ -2254,7 +2271,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B4" s="9" t="s">
         <v>17</v>
       </c>
@@ -2280,7 +2297,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5" s="8" t="s">
         <v>18</v>
       </c>
@@ -2306,7 +2323,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" s="9" t="s">
         <v>20</v>
       </c>
@@ -2332,7 +2349,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7" s="9" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
Ops has been updated
Ops has been updated
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/DailyStatusTracker.xlsx
+++ b/Offline/BusinessManagement/DailyStatusTracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BCBB4D5-D884-403A-9B18-7D92A8FA165F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF0B09D4-3F3F-4F83-8036-CA54463886A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,18 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tracker!$A$1:$H$31</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -939,7 +950,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="11">
         <v>1</v>
       </c>
@@ -1002,7 +1013,7 @@
       </c>
       <c r="G4" s="10"/>
     </row>
-    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="11">
         <v>4</v>
       </c>
@@ -1023,7 +1034,7 @@
       </c>
       <c r="G5" s="10"/>
     </row>
-    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="11">
         <v>5</v>
       </c>
@@ -1046,7 +1057,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="11">
         <v>6</v>
       </c>
@@ -1067,7 +1078,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="11">
         <v>7</v>
       </c>
@@ -1113,7 +1124,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="11">
         <v>9</v>
       </c>
@@ -1289,7 +1300,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="11">
         <v>17</v>
       </c>
@@ -1355,7 +1366,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="11">
         <v>20</v>
       </c>
@@ -1378,7 +1389,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="11">
         <v>21</v>
       </c>
@@ -1401,7 +1412,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="11">
         <v>22</v>
       </c>
@@ -1424,7 +1435,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="11">
         <v>23</v>
       </c>
@@ -1447,7 +1458,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="25" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" s="13" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="11">
         <v>24</v>
       </c>
@@ -1470,7 +1481,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="11">
         <v>25</v>
       </c>
@@ -1494,7 +1505,7 @@
       </c>
       <c r="H26" s="13"/>
     </row>
-    <row r="27" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" s="13" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="11">
         <v>26</v>
       </c>
@@ -1514,7 +1525,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="11">
         <v>27</v>
       </c>
@@ -1535,7 +1546,7 @@
       </c>
       <c r="G28" s="15"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="11">
         <v>28</v>
       </c>
@@ -1558,7 +1569,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="11">
         <v>29</v>
       </c>
@@ -1581,7 +1592,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="11">
         <v>30</v>
       </c>
@@ -1606,9 +1617,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:H31" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <filterColumn colId="3">
+    <filterColumn colId="5">
       <filters>
-        <filter val="Debashish"/>
+        <filter val="WIP"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Daily Status Tracker Updated
Daily Status Tracker Updated
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/DailyStatusTracker.xlsx
+++ b/Offline/BusinessManagement/DailyStatusTracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF0B09D4-3F3F-4F83-8036-CA54463886A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE6DBDF7-DC36-4230-A5FD-168E21C28787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -572,7 +572,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -589,17 +589,28 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -904,12 +915,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G25" sqref="G25"/>
+      <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -951,679 +961,706 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="11">
+      <c r="A2" s="10">
         <v>1</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="10">
-        <v>5</v>
-      </c>
-      <c r="F2" s="10" t="s">
+      <c r="E2" s="12">
+        <v>5</v>
+      </c>
+      <c r="F2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="10"/>
-    </row>
-    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="11">
+      <c r="G2" s="12"/>
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="10">
         <v>2</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="10">
-        <v>5</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="10"/>
-    </row>
-    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="11">
+      <c r="E3" s="12">
+        <v>5</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="12"/>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="10">
         <v>3</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="10">
-        <v>5</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" s="10"/>
+      <c r="E4" s="12">
+        <v>5</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="12"/>
+      <c r="H4" s="3"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="11">
+      <c r="A5" s="10">
         <v>4</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="10">
-        <v>5</v>
-      </c>
-      <c r="F5" s="10" t="s">
+      <c r="E5" s="12">
+        <v>5</v>
+      </c>
+      <c r="F5" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="10"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="11">
-        <v>5</v>
-      </c>
-      <c r="B6" s="16" t="s">
+      <c r="A6" s="10">
+        <v>5</v>
+      </c>
+      <c r="B6" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="10">
-        <v>5</v>
-      </c>
-      <c r="F6" s="10" t="s">
+      <c r="E6" s="12">
+        <v>5</v>
+      </c>
+      <c r="F6" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="12" t="s">
         <v>125</v>
       </c>
+      <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="11">
+      <c r="A7" s="10">
         <v>6</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="10">
-        <v>5</v>
-      </c>
-      <c r="F7" s="10" t="s">
+      <c r="E7" s="12">
+        <v>5</v>
+      </c>
+      <c r="F7" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="10"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="11">
+      <c r="A8" s="10">
         <v>7</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="10">
-        <v>5</v>
-      </c>
-      <c r="F8" s="10" t="s">
+      <c r="E8" s="12">
+        <v>5</v>
+      </c>
+      <c r="F8" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="G8" s="12" t="s">
         <v>103</v>
       </c>
+      <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:8" ht="259.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="11">
+      <c r="A9" s="13">
         <v>8</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="10">
-        <v>5</v>
-      </c>
-      <c r="F9" s="10" t="s">
+      <c r="E9" s="12">
+        <v>5</v>
+      </c>
+      <c r="F9" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="14" t="s">
         <v>130</v>
       </c>
+      <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="11">
+      <c r="A10" s="10">
         <v>9</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="10">
-        <v>5</v>
-      </c>
-      <c r="F10" s="10" t="s">
+      <c r="E10" s="12">
+        <v>5</v>
+      </c>
+      <c r="F10" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="10"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="11">
+      <c r="A11" s="10">
         <v>10</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="10">
-        <v>5</v>
-      </c>
-      <c r="F11" s="10" t="s">
+      <c r="E11" s="12">
+        <v>5</v>
+      </c>
+      <c r="F11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="G11" s="12" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="11">
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="10">
         <v>11</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="10">
-        <v>5</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="G12" s="10" t="s">
+      <c r="E12" s="12">
+        <v>5</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12" s="12" t="s">
         <v>93</v>
       </c>
+      <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="11">
+      <c r="A13" s="10">
         <v>12</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="E13" s="10">
-        <v>5</v>
-      </c>
-      <c r="F13" s="10" t="s">
+      <c r="E13" s="15">
+        <v>5</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="H13" s="3"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="10">
+        <v>13</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" s="12">
+        <v>5</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="10">
+        <v>14</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="12">
+        <v>4</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="10">
+        <v>15</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="12">
+        <v>3</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="H16" s="3"/>
+    </row>
+    <row r="17" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="10">
+        <v>16</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="12">
+        <v>3</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="10">
+        <v>17</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="12">
+        <v>5</v>
+      </c>
+      <c r="F18" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="G13" s="6" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="11">
+      <c r="G18" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="H18" s="3"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="10">
+        <v>18</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" s="12">
+        <v>3</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="10">
+        <v>19</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" s="12">
+        <v>5</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="H20" s="3"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="10">
+        <v>20</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="E21" s="18">
+        <v>5</v>
+      </c>
+      <c r="F21" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="G21" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="H21" s="3"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="10">
+        <v>21</v>
+      </c>
+      <c r="B22" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="C14" s="10" t="s">
+      <c r="C22" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="12">
+        <v>3</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="H22" s="3"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="10">
+        <v>22</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="12">
+        <v>3</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="H23" s="3"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="10">
+        <v>23</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D24" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="10">
-        <v>5</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="11">
-        <v>14</v>
-      </c>
-      <c r="B15" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="C15" s="10" t="s">
+      <c r="E24" s="12">
+        <v>2</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G24" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="H24" s="3"/>
+    </row>
+    <row r="25" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="21">
+        <v>24</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E25" s="15">
+        <v>5</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="G25" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="H25" s="22"/>
+    </row>
+    <row r="26" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="21">
+        <v>25</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E26" s="15">
+        <v>5</v>
+      </c>
+      <c r="F26" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="G26" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="H26" s="22"/>
+    </row>
+    <row r="27" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="21">
+        <v>26</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="C27" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="D15" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" s="10">
-        <v>4</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="11">
-        <v>15</v>
-      </c>
-      <c r="B16" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="C16" s="10" t="s">
+      <c r="D27" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E27" s="15">
+        <v>5</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="G27" s="19"/>
+      <c r="H27" s="22"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="10">
+        <v>27</v>
+      </c>
+      <c r="B28" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="C28" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="D16" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="10">
-        <v>3</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="G16" s="10" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="11">
-        <v>16</v>
-      </c>
-      <c r="B17" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" s="10">
-        <v>3</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="11">
-        <v>17</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" s="10">
-        <v>5</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="G18" s="10" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="11">
-        <v>18</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="E19" s="10">
-        <v>3</v>
-      </c>
-      <c r="F19" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="11">
-        <v>19</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="D20" s="10" t="s">
+      <c r="D28" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="E20" s="10">
-        <v>5</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="G20" s="10" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="11">
-        <v>20</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="D21" s="15" t="s">
+      <c r="E28" s="18">
+        <v>5</v>
+      </c>
+      <c r="F28" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="G28" s="18"/>
+      <c r="H28" s="3"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="10">
+        <v>28</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="D29" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="E21" s="15">
-        <v>5</v>
-      </c>
-      <c r="F21" s="15" t="s">
+      <c r="E29" s="18">
+        <v>5</v>
+      </c>
+      <c r="F29" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="G21" s="15" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="11">
-        <v>21</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E22" s="10">
-        <v>3</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="G22" s="10" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="11">
-        <v>22</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E23" s="10">
-        <v>3</v>
-      </c>
-      <c r="F23" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="G23" s="10" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="11">
-        <v>23</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C24" s="10" t="s">
+      <c r="G29" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="H29" s="3"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="10">
+        <v>29</v>
+      </c>
+      <c r="B30" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="C30" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="D24" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="E24" s="10">
-        <v>2</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="G24" s="10" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" s="13" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="11">
-        <v>24</v>
-      </c>
-      <c r="B25" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="D25" s="12" t="s">
+      <c r="D30" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="E25" s="12">
-        <v>5</v>
-      </c>
-      <c r="F25" s="12" t="s">
+      <c r="E30" s="18">
+        <v>5</v>
+      </c>
+      <c r="F30" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="G25" s="12" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="11">
-        <v>25</v>
-      </c>
-      <c r="B26" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="D26" s="12" t="s">
+      <c r="G30" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="H30" s="3"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="10">
+        <v>30</v>
+      </c>
+      <c r="B31" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="D31" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="E26" s="12">
-        <v>5</v>
-      </c>
-      <c r="F26" s="12" t="s">
+      <c r="E31" s="18">
+        <v>5</v>
+      </c>
+      <c r="F31" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="G26" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="H26" s="13"/>
-    </row>
-    <row r="27" spans="1:8" s="13" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="11">
-        <v>26</v>
-      </c>
-      <c r="B27" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="D27" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="E27" s="12">
-        <v>5</v>
-      </c>
-      <c r="F27" s="12" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="11">
-        <v>27</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="C28" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="D28" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E28" s="15">
-        <v>5</v>
-      </c>
-      <c r="F28" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="G28" s="15"/>
-    </row>
-    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="11">
-        <v>28</v>
-      </c>
-      <c r="B29" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="C29" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="D29" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E29" s="15">
-        <v>5</v>
-      </c>
-      <c r="F29" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="G29" s="15" t="s">
+      <c r="G31" s="18" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="11">
-        <v>29</v>
-      </c>
-      <c r="B30" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="C30" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="D30" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E30" s="15">
-        <v>5</v>
-      </c>
-      <c r="F30" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="G30" s="15" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="11">
-        <v>30</v>
-      </c>
-      <c r="B31" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="C31" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="D31" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E31" s="15">
-        <v>5</v>
-      </c>
-      <c r="F31" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="G31" s="15" t="s">
-        <v>131</v>
-      </c>
+      <c r="H31" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H31" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <filterColumn colId="5">
-      <filters>
-        <filter val="WIP"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
-  <dataValidations count="1">
+  <autoFilter ref="A1:H31" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1048576" xr:uid="{F694DCE3-45FE-4850-A54A-8379FCD46E21}">
       <formula1>"Todo,WIP,Done"</formula1>
     </dataValidation>

</xml_diff>

<commit_message>
Daily Status Tracker and Ops checked in
Daily Status Tracker and Ops checked in
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/DailyStatusTracker.xlsx
+++ b/Offline/BusinessManagement/DailyStatusTracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE6DBDF7-DC36-4230-A5FD-168E21C28787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E85B805D-F11A-4102-98FF-2EA837590267}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -572,7 +572,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -605,12 +605,6 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -919,7 +913,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1168,22 +1162,22 @@
       <c r="A11" s="10">
         <v>10</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="12">
-        <v>5</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="G11" s="12" t="s">
+      <c r="E11" s="15">
+        <v>5</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="G11" s="15" t="s">
         <v>107</v>
       </c>
       <c r="H11" s="3"/>
@@ -1231,7 +1225,7 @@
       <c r="F13" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="G13" s="20" t="s">
+      <c r="G13" s="19" t="s">
         <v>137</v>
       </c>
       <c r="H13" s="3"/>
@@ -1304,7 +1298,7 @@
       </c>
       <c r="H16" s="3"/>
     </row>
-    <row r="17" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="10">
         <v>16</v>
       </c>
@@ -1494,8 +1488,8 @@
       </c>
       <c r="H24" s="3"/>
     </row>
-    <row r="25" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="21">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="10">
         <v>24</v>
       </c>
       <c r="B25" s="15" t="s">
@@ -1516,10 +1510,10 @@
       <c r="G25" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="H25" s="22"/>
-    </row>
-    <row r="26" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="21">
+      <c r="H25" s="3"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="10">
         <v>25</v>
       </c>
       <c r="B26" s="15" t="s">
@@ -1540,10 +1534,10 @@
       <c r="G26" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="H26" s="22"/>
-    </row>
-    <row r="27" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="21">
+      <c r="H26" s="3"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="10">
         <v>26</v>
       </c>
       <c r="B27" s="15" t="s">
@@ -1562,7 +1556,7 @@
         <v>119</v>
       </c>
       <c r="G27" s="19"/>
-      <c r="H27" s="22"/>
+      <c r="H27" s="3"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="10">
@@ -1660,7 +1654,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:H31" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1048576" xr:uid="{F694DCE3-45FE-4850-A54A-8379FCD46E21}">
       <formula1>"Todo,WIP,Done"</formula1>
     </dataValidation>

</xml_diff>

<commit_message>
Update Daily Status Tracker
Update Daily Status Tracker
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/DailyStatusTracker.xlsx
+++ b/Offline/BusinessManagement/DailyStatusTracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E85B805D-F11A-4102-98FF-2EA837590267}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7742B29-685E-410A-BE54-F350F556BE30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -912,7 +912,7 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Daily status tracker updated with Antech issues
Daily status tracker updated with Antech issues
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/DailyStatusTracker.xlsx
+++ b/Offline/BusinessManagement/DailyStatusTracker.xlsx
@@ -3,14 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2746BEE-2303-4D03-B47F-BF8A5F42E84D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB5A13C4-C8EF-49E2-A9A4-DF9CC8EF5A36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tracker" sheetId="1" r:id="rId1"/>
     <sheet name="MockTest" sheetId="3" r:id="rId2"/>
-    <sheet name="WorkDays" sheetId="2" r:id="rId3"/>
+    <sheet name="Antech-Issues" sheetId="4" r:id="rId3"/>
+    <sheet name="WorkDays" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tracker!$A$1:$H$29</definedName>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="145">
   <si>
     <t>Item Number</t>
   </si>
@@ -450,6 +451,27 @@
   </si>
   <si>
     <t>CRM calls: Just dial to Urban Pro</t>
+  </si>
+  <si>
+    <t>Opening Hours should be 10 AM to 7 PM.</t>
+  </si>
+  <si>
+    <t>Antech</t>
+  </si>
+  <si>
+    <t>Address of our institute should be : N 1/25, Kunal Road,Patuli, Kolkata - 700094</t>
+  </si>
+  <si>
+    <t>In Appointments: wa.me area, there should be whats app icon.</t>
+  </si>
+  <si>
+    <t>There is no place for giving review comments</t>
+  </si>
+  <si>
+    <t>On pressing Website button the page should redirect to google.anodiam.mybusiness.site</t>
+  </si>
+  <si>
+    <t>The outside photo (360 degree) of our institute should be proper with banners and no blury images</t>
   </si>
 </sst>
 </file>
@@ -894,24 +916,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.33203125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="46.73046875" customWidth="1"/>
+    <col min="2" max="2" width="46.77734375" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.6640625" customWidth="1"/>
-    <col min="5" max="5" width="9.1328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="67.73046875" customWidth="1"/>
-    <col min="8" max="8" width="15.796875" customWidth="1"/>
+    <col min="7" max="7" width="67.77734375" customWidth="1"/>
+    <col min="8" max="8" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -937,7 +959,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="10">
         <v>1</v>
       </c>
@@ -959,7 +981,7 @@
       <c r="G2" s="12"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="10">
         <v>2</v>
       </c>
@@ -981,7 +1003,7 @@
       <c r="G3" s="12"/>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="10">
         <v>3</v>
       </c>
@@ -1003,7 +1025,7 @@
       <c r="G4" s="12"/>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="10">
         <v>4</v>
       </c>
@@ -1025,7 +1047,7 @@
       <c r="G5" s="12"/>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="10">
         <v>5</v>
       </c>
@@ -1049,7 +1071,7 @@
       </c>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="10">
         <v>6</v>
       </c>
@@ -1071,7 +1093,7 @@
       <c r="G7" s="12"/>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="10">
         <v>7</v>
       </c>
@@ -1093,7 +1115,7 @@
       <c r="G8" s="12"/>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10">
         <v>8</v>
       </c>
@@ -1117,7 +1139,7 @@
       </c>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -1139,7 +1161,7 @@
       <c r="G10" s="12"/>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -1163,7 +1185,7 @@
       </c>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -1187,7 +1209,7 @@
       </c>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -1209,7 +1231,7 @@
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="10">
         <v>13</v>
       </c>
@@ -1231,7 +1253,7 @@
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="10">
         <v>14</v>
       </c>
@@ -1255,7 +1277,7 @@
       </c>
       <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="10">
         <v>15</v>
       </c>
@@ -1279,7 +1301,7 @@
       </c>
       <c r="H16" s="3"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="10">
         <v>16</v>
       </c>
@@ -1303,7 +1325,7 @@
       </c>
       <c r="H17" s="3"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="10">
         <v>17</v>
       </c>
@@ -1327,7 +1349,7 @@
       </c>
       <c r="H18" s="3"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="10">
         <v>18</v>
       </c>
@@ -1351,7 +1373,7 @@
       </c>
       <c r="H19" s="3"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="10">
         <v>19</v>
       </c>
@@ -1375,7 +1397,7 @@
       </c>
       <c r="H20" s="3"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="10">
         <v>20</v>
       </c>
@@ -1399,7 +1421,7 @@
       </c>
       <c r="H21" s="3"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="10">
         <v>21</v>
       </c>
@@ -1423,7 +1445,7 @@
       </c>
       <c r="H22" s="3"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="10">
         <v>22</v>
       </c>
@@ -1447,7 +1469,7 @@
       </c>
       <c r="H23" s="3"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="10">
         <v>23</v>
       </c>
@@ -1469,7 +1491,7 @@
       <c r="G24" s="18"/>
       <c r="H24" s="3"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="10">
         <v>24</v>
       </c>
@@ -1493,7 +1515,7 @@
       </c>
       <c r="H25" s="3"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="10">
         <v>25</v>
       </c>
@@ -1515,7 +1537,7 @@
       <c r="G26" s="17"/>
       <c r="H26" s="3"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="10">
         <v>26</v>
       </c>
@@ -1539,7 +1561,7 @@
       </c>
       <c r="H27" s="3"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="10">
         <v>27</v>
       </c>
@@ -1563,7 +1585,7 @@
       </c>
       <c r="H28" s="3"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="10">
         <v>28</v>
       </c>
@@ -1587,7 +1609,7 @@
       </c>
       <c r="H29" s="3"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="10">
         <v>29</v>
       </c>
@@ -1609,7 +1631,7 @@
       <c r="G30" s="17"/>
       <c r="H30" s="3"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="10">
         <v>30</v>
       </c>
@@ -1652,9 +1674,9 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>23</v>
       </c>
@@ -1674,7 +1696,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>24</v>
       </c>
@@ -1694,7 +1716,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>25</v>
       </c>
@@ -1714,7 +1736,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>26</v>
       </c>
@@ -1734,7 +1756,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>20</v>
       </c>
@@ -1754,7 +1776,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>21</v>
       </c>
@@ -1774,7 +1796,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>28</v>
       </c>
@@ -1785,7 +1807,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>29</v>
       </c>
@@ -1796,7 +1818,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>30</v>
       </c>
@@ -1807,7 +1829,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>31</v>
       </c>
@@ -1818,7 +1840,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>32</v>
       </c>
@@ -1829,7 +1851,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>33</v>
       </c>
@@ -1840,7 +1862,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>34</v>
       </c>
@@ -1851,7 +1873,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>35</v>
       </c>
@@ -1862,7 +1884,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>36</v>
       </c>
@@ -1873,7 +1895,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>37</v>
       </c>
@@ -1884,7 +1906,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>38</v>
       </c>
@@ -1895,7 +1917,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="409.5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>39</v>
       </c>
@@ -1906,7 +1928,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>40</v>
       </c>
@@ -1917,7 +1939,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>41</v>
       </c>
@@ -1928,7 +1950,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <v>42</v>
       </c>
@@ -1939,7 +1961,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>43</v>
       </c>
@@ -1950,7 +1972,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
         <v>44</v>
       </c>
@@ -1961,7 +1983,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
         <v>45</v>
       </c>
@@ -1972,7 +1994,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
         <v>46</v>
       </c>
@@ -1983,7 +2005,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
         <v>47</v>
       </c>
@@ -1994,7 +2016,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="5">
         <v>48</v>
       </c>
@@ -2005,7 +2027,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="5">
         <v>49</v>
       </c>
@@ -2016,7 +2038,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
         <v>50</v>
       </c>
@@ -2027,7 +2049,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="5">
         <v>51</v>
       </c>
@@ -2038,7 +2060,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="5">
         <v>52</v>
       </c>
@@ -2049,7 +2071,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="5">
         <v>53</v>
       </c>
@@ -2060,7 +2082,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="5">
         <v>54</v>
       </c>
@@ -2071,7 +2093,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="5">
         <v>55</v>
       </c>
@@ -2082,7 +2104,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="5">
         <v>56</v>
       </c>
@@ -2093,7 +2115,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="5">
         <v>57</v>
       </c>
@@ -2104,7 +2126,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="5">
         <v>58</v>
       </c>
@@ -2115,7 +2137,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="5">
         <v>59</v>
       </c>
@@ -2126,7 +2148,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="5">
         <v>60</v>
       </c>
@@ -2137,7 +2159,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="5">
         <v>61</v>
       </c>
@@ -2148,7 +2170,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="5">
         <v>62</v>
       </c>
@@ -2159,7 +2181,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="5">
         <v>63</v>
       </c>
@@ -2170,7 +2192,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="5">
         <v>64</v>
       </c>
@@ -2181,7 +2203,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="5">
         <v>65</v>
       </c>
@@ -2192,7 +2214,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="5">
         <v>66</v>
       </c>
@@ -2203,7 +2225,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="5">
         <v>67</v>
       </c>
@@ -2214,7 +2236,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="5">
         <v>69</v>
       </c>
@@ -2225,7 +2247,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="5">
         <v>70</v>
       </c>
@@ -2236,7 +2258,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="5">
         <v>71</v>
       </c>
@@ -2247,7 +2269,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="5">
         <v>72</v>
       </c>
@@ -2258,7 +2280,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="5">
         <v>73</v>
       </c>
@@ -2269,7 +2291,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="5">
         <v>74</v>
       </c>
@@ -2280,7 +2302,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="5">
         <v>75</v>
       </c>
@@ -2297,6 +2319,182 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62E6E54B-2AD5-4B89-AEAC-D087C44BF4B1}">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.21875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.21875" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="7" max="7" width="10.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" t="s">
+        <v>139</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>142</v>
+      </c>
+      <c r="C6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D6" t="s">
+        <v>139</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>143</v>
+      </c>
+      <c r="C7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D7" t="s">
+        <v>139</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1048576" xr:uid="{360E118C-F521-4CC7-8556-EFA9418D197E}">
+      <formula1>"Todo,WIP,Done"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576" xr:uid="{A1101A09-0BF8-4916-A084-6A46F4BC7A80}">
+      <formula1>"Marketing"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576" xr:uid="{051203AA-A044-47B3-ADD5-39B3C5409E6D}">
+      <formula1>"Antech,Anirban,Debashish,Sayan,Rahul"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:I7"/>
   <sheetViews>
@@ -2304,18 +2502,18 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.19921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="7.46484375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.19921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.19921875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.46484375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.86328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.46484375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>16</v>
       </c>
@@ -2341,7 +2539,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B3" s="8" t="s">
         <v>30</v>
       </c>
@@ -2367,7 +2565,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B4" s="9" t="s">
         <v>17</v>
       </c>
@@ -2393,7 +2591,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5" s="8" t="s">
         <v>18</v>
       </c>
@@ -2419,7 +2617,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" s="9" t="s">
         <v>20</v>
       </c>
@@ -2445,7 +2643,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7" s="9" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
excel sheet related to expense
excel sheet related to expense
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/DailyStatusTracker.xlsx
+++ b/Offline/BusinessManagement/DailyStatusTracker.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E47B6D29-659E-48E4-9AA1-8563D0EE51A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8190D617-A839-473E-947C-CAF0858468F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tracker" sheetId="1" r:id="rId1"/>
@@ -927,9 +927,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1009,7 +1009,7 @@
         <v>5</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>8</v>
+        <v>115</v>
       </c>
       <c r="G3" s="12"/>
       <c r="H3" s="3"/>
@@ -1031,7 +1031,7 @@
         <v>5</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>8</v>
+        <v>115</v>
       </c>
       <c r="G4" s="12"/>
       <c r="H4" s="3"/>
@@ -1172,7 +1172,7 @@
       <c r="G10" s="12"/>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -1189,7 +1189,7 @@
         <v>5</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G11" s="13" t="s">
         <v>136</v>
@@ -2333,7 +2333,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62E6E54B-2AD5-4B89-AEAC-D087C44BF4B1}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Daily Status Tracker and AI school colleges done
Daily Status Tracker and AI school colleges done
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/DailyStatusTracker.xlsx
+++ b/Offline/BusinessManagement/DailyStatusTracker.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8190D617-A839-473E-947C-CAF0858468F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E197E43-FAA5-427A-9505-9CD1F35606DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="563" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tracker" sheetId="1" r:id="rId1"/>
@@ -400,9 +400,6 @@
     <t>Consilidate School and College marketing sheets into one workbook</t>
   </si>
   <si>
-    <t>Check Just Dial daily. Transfer to Urban Pro</t>
-  </si>
-  <si>
     <t>Classplus: Website first screen not responsive</t>
   </si>
   <si>
@@ -483,6 +480,9 @@
   </si>
   <si>
     <t>The outside photo (360 degree) of our institute should be proper with banners and no blury images</t>
+  </si>
+  <si>
+    <t>Check Just Dial daily. Transfer to Urban Pro. Just Dial email Id : kolkata@justdial.com</t>
   </si>
 </sst>
 </file>
@@ -927,9 +927,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1041,7 +1041,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>91</v>
@@ -1087,7 +1087,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>91</v>
@@ -1126,7 +1126,7 @@
       <c r="G8" s="12"/>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="262.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10">
         <v>8</v>
       </c>
@@ -1146,7 +1146,7 @@
         <v>8</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H9" s="3"/>
     </row>
@@ -1155,7 +1155,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>92</v>
@@ -1177,7 +1177,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>92</v>
@@ -1192,7 +1192,7 @@
         <v>8</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H11" s="3"/>
     </row>
@@ -1225,7 +1225,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>91</v>
@@ -1247,7 +1247,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>92</v>
@@ -1293,7 +1293,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C16" s="12" t="s">
         <v>94</v>
@@ -1308,7 +1308,7 @@
         <v>8</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>122</v>
+        <v>144</v>
       </c>
       <c r="H16" s="3"/>
     </row>
@@ -1522,7 +1522,7 @@
         <v>115</v>
       </c>
       <c r="G25" s="18" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H25" s="3"/>
     </row>
@@ -1553,7 +1553,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C27" s="17" t="s">
         <v>91</v>
@@ -1568,7 +1568,7 @@
         <v>115</v>
       </c>
       <c r="G27" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H27" s="3"/>
     </row>
@@ -1577,7 +1577,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C28" s="17" t="s">
         <v>91</v>
@@ -1592,7 +1592,7 @@
         <v>115</v>
       </c>
       <c r="G28" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H28" s="3"/>
     </row>
@@ -1601,7 +1601,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C29" s="17" t="s">
         <v>91</v>
@@ -1616,7 +1616,7 @@
         <v>115</v>
       </c>
       <c r="G29" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H29" s="3"/>
     </row>
@@ -1662,7 +1662,7 @@
         <v>115</v>
       </c>
       <c r="G31" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H31" s="3"/>
     </row>
@@ -1681,15 +1681,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F24168E-DBD7-4361-AEEA-D57845BDFBC0}">
   <dimension ref="A2:F54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="145.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="76" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>36</v>
@@ -1709,7 +1714,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>37</v>
@@ -1729,7 +1734,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>38</v>
@@ -1749,7 +1754,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>33</v>
@@ -1769,7 +1774,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>39</v>
@@ -1789,7 +1794,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>42</v>
@@ -1809,7 +1814,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>43</v>
@@ -1820,7 +1825,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>44</v>
@@ -1831,7 +1836,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>45</v>
@@ -1842,7 +1847,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>46</v>
@@ -1853,7 +1858,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>47</v>
@@ -1864,7 +1869,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>48</v>
@@ -1875,7 +1880,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>49</v>
@@ -1886,7 +1891,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>50</v>
@@ -1897,7 +1902,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>51</v>
@@ -1908,7 +1913,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>88</v>
@@ -1919,7 +1924,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>89</v>
@@ -1928,9 +1933,9 @@
         <v>96</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>77</v>
@@ -1941,7 +1946,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>52</v>
@@ -1952,7 +1957,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>53</v>
@@ -1963,7 +1968,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>54</v>
@@ -1974,7 +1979,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>55</v>
@@ -1985,7 +1990,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>56</v>
@@ -1996,7 +2001,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>57</v>
@@ -2007,7 +2012,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>58</v>
@@ -2018,7 +2023,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>59</v>
@@ -2029,7 +2034,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="5">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>60</v>
@@ -2040,7 +2045,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="5">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>61</v>
@@ -2051,7 +2056,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>62</v>
@@ -2062,7 +2067,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="5">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>63</v>
@@ -2073,7 +2078,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="5">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>64</v>
@@ -2084,7 +2089,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="5">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>65</v>
@@ -2095,7 +2100,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="5">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>66</v>
@@ -2106,7 +2111,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="5">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>67</v>
@@ -2117,7 +2122,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="5">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>68</v>
@@ -2128,7 +2133,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="5">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="B37" s="6" t="s">
         <v>69</v>
@@ -2139,7 +2144,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="5">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>70</v>
@@ -2150,7 +2155,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="5">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="B39" s="6" t="s">
         <v>71</v>
@@ -2161,7 +2166,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="5">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="B40" s="6" t="s">
         <v>72</v>
@@ -2172,7 +2177,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="5">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="B41" s="6" t="s">
         <v>73</v>
@@ -2183,7 +2188,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="5">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="B42" s="6" t="s">
         <v>74</v>
@@ -2194,7 +2199,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="5">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="B43" s="6" t="s">
         <v>75</v>
@@ -2205,7 +2210,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="5">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="B44" s="6" t="s">
         <v>76</v>
@@ -2216,7 +2221,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="5">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>78</v>
@@ -2227,7 +2232,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="5">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="B46" s="6" t="s">
         <v>79</v>
@@ -2238,7 +2243,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="5">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="B47" s="6" t="s">
         <v>80</v>
@@ -2249,7 +2254,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="5">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="B48" s="6" t="s">
         <v>81</v>
@@ -2260,7 +2265,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="5">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>82</v>
@@ -2271,7 +2276,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="5">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="B50" s="6" t="s">
         <v>83</v>
@@ -2282,7 +2287,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="5">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="B51" s="6" t="s">
         <v>84</v>
@@ -2293,7 +2298,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="5">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="B52" s="6" t="s">
         <v>85</v>
@@ -2304,7 +2309,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="5">
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="B53" s="6" t="s">
         <v>86</v>
@@ -2315,7 +2320,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="5">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="B54" s="6" t="s">
         <v>87</v>
@@ -2374,13 +2379,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C2" t="s">
         <v>91</v>
       </c>
       <c r="D2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E2">
         <v>5</v>
@@ -2394,13 +2399,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C3" t="s">
         <v>91</v>
       </c>
       <c r="D3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E3">
         <v>5</v>
@@ -2414,13 +2419,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C4" t="s">
         <v>91</v>
       </c>
       <c r="D4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E4">
         <v>5</v>
@@ -2434,13 +2439,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C5" t="s">
         <v>91</v>
       </c>
       <c r="D5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E5">
         <v>5</v>
@@ -2454,13 +2459,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C6" t="s">
         <v>91</v>
       </c>
       <c r="D6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E6">
         <v>5</v>
@@ -2474,13 +2479,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C7" t="s">
         <v>91</v>
       </c>
       <c r="D7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E7">
         <v>5</v>

</xml_diff>

<commit_message>
Updated Daily Status Tracker sheet
Updated Daily Status Tracker sheet
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/DailyStatusTracker.xlsx
+++ b/Offline/BusinessManagement/DailyStatusTracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7DCAF34-714E-42DB-B2AC-14D2AB447854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C01CFC-E491-42DF-BE07-28FA6896B030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="563" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="179">
   <si>
     <t>Item Number</t>
   </si>
@@ -557,6 +557,9 @@
   </si>
   <si>
     <t>5. Must have a button "Visit anodiam.com website": upon clicking it will open anodiam.com &gt;&gt; classplus/YOWWA website</t>
+  </si>
+  <si>
+    <t>Given Avishek to review 16 chapters of Maths. After positive feedback course will be uploaded.</t>
   </si>
 </sst>
 </file>
@@ -665,7 +668,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -704,8 +707,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1010,11 +1011,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1055,7 +1057,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10">
         <v>1</v>
       </c>
@@ -1077,7 +1079,7 @@
       <c r="G2" s="12"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10">
         <v>2</v>
       </c>
@@ -1099,7 +1101,7 @@
       <c r="G3" s="14"/>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10">
         <v>3</v>
       </c>
@@ -1121,7 +1123,7 @@
       <c r="G4" s="14"/>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10">
         <v>4</v>
       </c>
@@ -1143,7 +1145,7 @@
       <c r="G5" s="12"/>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10">
         <v>5</v>
       </c>
@@ -1165,7 +1167,7 @@
       <c r="G6" s="12"/>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10">
         <v>6</v>
       </c>
@@ -1187,7 +1189,7 @@
       <c r="G7" s="12"/>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10">
         <v>7</v>
       </c>
@@ -1209,7 +1211,7 @@
       <c r="G8" s="14"/>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10">
         <v>8</v>
       </c>
@@ -1257,7 +1259,7 @@
       </c>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -1281,11 +1283,11 @@
       </c>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10">
         <v>11</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="3" t="s">
         <v>124</v>
       </c>
       <c r="C12" s="12" t="s">
@@ -1307,7 +1309,7 @@
       <c r="A13" s="10">
         <v>12</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="12" t="s">
         <v>125</v>
       </c>
       <c r="C13" s="12" t="s">
@@ -1320,12 +1322,14 @@
         <v>4</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="G13" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>178</v>
+      </c>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10">
         <v>13</v>
       </c>
@@ -1349,7 +1353,7 @@
       </c>
       <c r="H14" s="3"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10">
         <v>14</v>
       </c>
@@ -1373,7 +1377,7 @@
       </c>
       <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10">
         <v>15</v>
       </c>
@@ -1397,11 +1401,11 @@
       </c>
       <c r="H16" s="3"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10">
         <v>16</v>
       </c>
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="12" t="s">
         <v>13</v>
       </c>
       <c r="C17" s="12" t="s">
@@ -1421,11 +1425,11 @@
       </c>
       <c r="H17" s="3"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10">
         <v>17</v>
       </c>
-      <c r="B18" s="22" t="s">
+      <c r="B18" s="12" t="s">
         <v>14</v>
       </c>
       <c r="C18" s="12" t="s">
@@ -1445,7 +1449,7 @@
       </c>
       <c r="H18" s="3"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="10">
         <v>18</v>
       </c>
@@ -1469,7 +1473,7 @@
       </c>
       <c r="H19" s="3"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="10">
         <v>19</v>
       </c>
@@ -1491,7 +1495,7 @@
       <c r="G20" s="14"/>
       <c r="H20" s="3"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="10">
         <v>20</v>
       </c>
@@ -1701,7 +1705,7 @@
       </c>
       <c r="H29" s="3"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="10">
         <v>29</v>
       </c>
@@ -1747,11 +1751,11 @@
       </c>
       <c r="H31" s="3"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="10">
         <v>31</v>
       </c>
-      <c r="B32" s="22" t="s">
+      <c r="B32" s="12" t="s">
         <v>142</v>
       </c>
       <c r="C32" s="12" t="s">
@@ -1769,7 +1773,13 @@
       <c r="G32" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H32" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:H32" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="Debashish"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1048576" xr:uid="{F694DCE3-45FE-4850-A54A-8379FCD46E21}">
       <formula1>"Todo,WIP,Done"</formula1>

</xml_diff>

<commit_message>
Update Daily Tracker Status
Update Daily Tracker Status
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/DailyStatusTracker.xlsx
+++ b/Offline/BusinessManagement/DailyStatusTracker.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23B36576-2F1B-4A18-AAA1-95693D3F72E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D646439-8FCD-4CB0-A1F7-F13C21996130}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="563" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="563" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tracker" sheetId="1" r:id="rId1"/>
@@ -1047,16 +1047,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.109375" style="5" customWidth="1"/>
     <col min="2" max="2" width="53.77734375" customWidth="1"/>
-    <col min="3" max="3" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.6640625" customWidth="1"/>
     <col min="5" max="5" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
@@ -2217,7 +2217,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62E6E54B-2AD5-4B89-AEAC-D087C44BF4B1}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
+    <sheetView zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Science is in progress
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/DailyStatusTracker.xlsx
+++ b/Offline/BusinessManagement/DailyStatusTracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE9F3F92-74DA-431A-AF6E-E020C1E626DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A1647EA-9850-436B-8FA6-BEF6CD356D61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="563" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1056,7 +1056,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
+      <selection pane="bottomLeft" activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Checked in the 5 Star Review file
Checked in the 5 Star Review file
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/DailyStatusTracker.xlsx
+++ b/Offline/BusinessManagement/DailyStatusTracker.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C43D1E3B-40A0-475C-9650-4E47A3094DB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7571100-1F9D-4727-82D8-594260CE1913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" tabRatio="563" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="563" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tracker" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="56">
   <si>
     <t>Item Description</t>
   </si>
@@ -186,9 +186,6 @@
     <t>Publish Java course materials on Anodiam platform</t>
   </si>
   <si>
-    <t>PPTs only for now at version 0.0.1.</t>
-  </si>
-  <si>
     <t>To be finished by 15-Feb</t>
   </si>
   <si>
@@ -196,6 +193,12 @@
   </si>
   <si>
     <t>Institution full name to be listed</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>PPTs only for now at version 0.0.1. Python for AI has been uploaded in Classplus website (Price given is Rs 1 as we will teach free)</t>
   </si>
 </sst>
 </file>
@@ -605,26 +608,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.19921875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="7.21875" style="2" customWidth="1"/>
     <col min="2" max="2" width="62" customWidth="1"/>
-    <col min="3" max="3" width="9.53125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.6640625" customWidth="1"/>
-    <col min="5" max="5" width="8.19921875" customWidth="1"/>
-    <col min="6" max="6" width="7.19921875" customWidth="1"/>
-    <col min="7" max="7" width="93.53125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.21875" customWidth="1"/>
+    <col min="6" max="6" width="7.21875" customWidth="1"/>
+    <col min="7" max="7" width="93.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>25</v>
       </c>
@@ -650,7 +654,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -674,7 +678,7 @@
       </c>
       <c r="H2" s="6"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -696,12 +700,12 @@
       <c r="G3" s="5"/>
       <c r="H3" s="6"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>14</v>
@@ -718,7 +722,7 @@
       <c r="G4" s="5"/>
       <c r="H4" s="6"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>5</v>
       </c>
@@ -742,7 +746,7 @@
       </c>
       <c r="H5" s="6"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>6</v>
       </c>
@@ -766,7 +770,7 @@
       </c>
       <c r="H6" s="6"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>7</v>
       </c>
@@ -790,7 +794,7 @@
       </c>
       <c r="H7" s="6"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>8</v>
       </c>
@@ -812,7 +816,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="6"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>9</v>
       </c>
@@ -834,7 +838,7 @@
       <c r="G9" s="1"/>
       <c r="H9" s="6"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>10</v>
       </c>
@@ -856,7 +860,7 @@
       <c r="G10" s="1"/>
       <c r="H10" s="6"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>11</v>
       </c>
@@ -878,7 +882,7 @@
       <c r="G11" s="5"/>
       <c r="H11" s="6"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>12</v>
       </c>
@@ -900,7 +904,7 @@
       <c r="G12" s="1"/>
       <c r="H12" s="6"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>13</v>
       </c>
@@ -922,7 +926,7 @@
       <c r="G13" s="5"/>
       <c r="H13" s="6"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>14</v>
       </c>
@@ -946,7 +950,7 @@
       </c>
       <c r="H14" s="6"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>15</v>
       </c>
@@ -970,7 +974,7 @@
       </c>
       <c r="H15" s="6"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>16</v>
       </c>
@@ -994,7 +998,7 @@
       </c>
       <c r="H16" s="6"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>17</v>
       </c>
@@ -1014,11 +1018,11 @@
         <v>6</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="H17" s="6"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>18</v>
       </c>
@@ -1035,14 +1039,14 @@
         <v>4</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>6</v>
+        <v>54</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H18" s="6"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>19</v>
       </c>
@@ -1062,11 +1066,11 @@
         <v>6</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H19" s="6"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>20</v>
       </c>
@@ -1090,7 +1094,7 @@
       </c>
       <c r="H20" s="6"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>21</v>
       </c>
@@ -1112,7 +1116,7 @@
       <c r="G21" s="5"/>
       <c r="H21" s="6"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>22</v>
       </c>
@@ -1136,7 +1140,7 @@
       </c>
       <c r="H22" s="6"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>23</v>
       </c>
@@ -1160,7 +1164,7 @@
       </c>
       <c r="H23" s="6"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>24</v>
       </c>
@@ -1184,7 +1188,7 @@
       </c>
       <c r="H24" s="6"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>25</v>
       </c>
@@ -1209,7 +1213,13 @@
       <c r="H25" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H25" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:H25" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="Rahul"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Todo,WIP,Done"</formula1>

</xml_diff>

<commit_message>
Daily Tracker checked in
Daily Tracker checked in
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/DailyStatusTracker.xlsx
+++ b/Offline/BusinessManagement/DailyStatusTracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7571100-1F9D-4727-82D8-594260CE1913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED1AF100-98A6-45CD-91F6-35C363CF877F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="563" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -608,7 +608,6 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
@@ -624,7 +623,7 @@
     <col min="4" max="4" width="9.6640625" customWidth="1"/>
     <col min="5" max="5" width="8.21875" customWidth="1"/>
     <col min="6" max="6" width="7.21875" customWidth="1"/>
-    <col min="7" max="7" width="93.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="114.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
   </cols>
   <sheetData>
@@ -678,7 +677,7 @@
       </c>
       <c r="H2" s="6"/>
     </row>
-    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -722,7 +721,7 @@
       <c r="G4" s="5"/>
       <c r="H4" s="6"/>
     </row>
-    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>5</v>
       </c>
@@ -770,7 +769,7 @@
       </c>
       <c r="H6" s="6"/>
     </row>
-    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>7</v>
       </c>
@@ -794,7 +793,7 @@
       </c>
       <c r="H7" s="6"/>
     </row>
-    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>8</v>
       </c>
@@ -816,7 +815,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="6"/>
     </row>
-    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>9</v>
       </c>
@@ -838,7 +837,7 @@
       <c r="G9" s="1"/>
       <c r="H9" s="6"/>
     </row>
-    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>10</v>
       </c>
@@ -860,7 +859,7 @@
       <c r="G10" s="1"/>
       <c r="H10" s="6"/>
     </row>
-    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>11</v>
       </c>
@@ -882,7 +881,7 @@
       <c r="G11" s="5"/>
       <c r="H11" s="6"/>
     </row>
-    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>12</v>
       </c>
@@ -904,7 +903,7 @@
       <c r="G12" s="1"/>
       <c r="H12" s="6"/>
     </row>
-    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>13</v>
       </c>
@@ -926,7 +925,7 @@
       <c r="G13" s="5"/>
       <c r="H13" s="6"/>
     </row>
-    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>14</v>
       </c>
@@ -974,7 +973,7 @@
       </c>
       <c r="H15" s="6"/>
     </row>
-    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>16</v>
       </c>
@@ -998,7 +997,7 @@
       </c>
       <c r="H16" s="6"/>
     </row>
-    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>17</v>
       </c>
@@ -1022,7 +1021,7 @@
       </c>
       <c r="H17" s="6"/>
     </row>
-    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>18</v>
       </c>
@@ -1094,7 +1093,7 @@
       </c>
       <c r="H20" s="6"/>
     </row>
-    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>21</v>
       </c>
@@ -1116,7 +1115,7 @@
       <c r="G21" s="5"/>
       <c r="H21" s="6"/>
     </row>
-    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>22</v>
       </c>
@@ -1140,7 +1139,7 @@
       </c>
       <c r="H22" s="6"/>
     </row>
-    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>23</v>
       </c>
@@ -1213,13 +1212,7 @@
       <c r="H25" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H25" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="Rahul"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:H25" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Todo,WIP,Done"</formula1>

</xml_diff>

<commit_message>
Daily Status Tracker Checked in
Daily Status Tracker Checked in
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/DailyStatusTracker.xlsx
+++ b/Offline/BusinessManagement/DailyStatusTracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED1AF100-98A6-45CD-91F6-35C363CF877F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E566BA79-09D6-4C38-BF78-FD14A0D3338A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="563" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -92,9 +92,6 @@
     <t>AI Internal Classes - Sayan</t>
   </si>
   <si>
-    <t>Pranay has been updated.</t>
-  </si>
-  <si>
     <t>SlNo</t>
   </si>
   <si>
@@ -199,6 +196,9 @@
   </si>
   <si>
     <t>PPTs only for now at version 0.0.1. Python for AI has been uploaded in Classplus website (Price given is Rs 1 as we will teach free)</t>
+  </si>
+  <si>
+    <t>Ashmita did not picked up the call.</t>
   </si>
 </sst>
 </file>
@@ -236,7 +236,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -246,6 +246,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -290,7 +296,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -304,6 +310,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -629,7 +636,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -658,7 +665,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>14</v>
@@ -673,7 +680,7 @@
         <v>6</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H2" s="6"/>
     </row>
@@ -682,13 +689,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E3" s="5">
         <v>5</v>
@@ -704,7 +711,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>14</v>
@@ -726,7 +733,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>15</v>
@@ -741,7 +748,7 @@
         <v>6</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H5" s="6"/>
     </row>
@@ -750,7 +757,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>14</v>
@@ -765,7 +772,7 @@
         <v>4</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H6" s="6"/>
     </row>
@@ -774,13 +781,13 @@
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E7" s="5">
         <v>5</v>
@@ -789,7 +796,7 @@
         <v>6</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H7" s="6"/>
     </row>
@@ -798,7 +805,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>14</v>
@@ -820,13 +827,13 @@
         <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>46</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>47</v>
       </c>
       <c r="E9" s="5">
         <v>5</v>
@@ -842,7 +849,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>14</v>
@@ -864,7 +871,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>14</v>
@@ -886,13 +893,13 @@
         <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E12" s="5">
         <v>5</v>
@@ -908,7 +915,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>15</v>
@@ -945,7 +952,7 @@
         <v>6</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H14" s="6"/>
     </row>
@@ -954,7 +961,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>15</v>
@@ -969,7 +976,7 @@
         <v>6</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H15" s="6"/>
     </row>
@@ -1002,7 +1009,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>15</v>
@@ -1017,7 +1024,7 @@
         <v>6</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H17" s="6"/>
     </row>
@@ -1026,22 +1033,22 @@
         <v>18</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E18" s="5">
         <v>4</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H18" s="6"/>
     </row>
@@ -1050,7 +1057,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>14</v>
@@ -1065,7 +1072,7 @@
         <v>6</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H19" s="6"/>
     </row>
@@ -1074,7 +1081,7 @@
         <v>20</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>16</v>
@@ -1089,7 +1096,7 @@
         <v>6</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H20" s="6"/>
     </row>
@@ -1098,7 +1105,7 @@
         <v>21</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>16</v>
@@ -1167,23 +1174,23 @@
       <c r="A24" s="3">
         <v>24</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E24" s="5">
+      <c r="E24" s="7">
         <v>3</v>
       </c>
-      <c r="F24" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>24</v>
+      <c r="F24" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>55</v>
       </c>
       <c r="H24" s="6"/>
     </row>

</xml_diff>

<commit_message>
Updated the daily status tracker
Updated the daily status tracker
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/DailyStatusTracker.xlsx
+++ b/Offline/BusinessManagement/DailyStatusTracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E566BA79-09D6-4C38-BF78-FD14A0D3338A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB53C0B-9180-46FC-B624-19442E0838F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="563" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -615,11 +615,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -684,7 +685,7 @@
       </c>
       <c r="H2" s="6"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -728,7 +729,7 @@
       <c r="G4" s="5"/>
       <c r="H4" s="6"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>5</v>
       </c>
@@ -769,14 +770,14 @@
         <v>5</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>42</v>
       </c>
       <c r="H6" s="6"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>7</v>
       </c>
@@ -800,7 +801,7 @@
       </c>
       <c r="H7" s="6"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>8</v>
       </c>
@@ -822,7 +823,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="6"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>9</v>
       </c>
@@ -844,7 +845,7 @@
       <c r="G9" s="1"/>
       <c r="H9" s="6"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>10</v>
       </c>
@@ -866,7 +867,7 @@
       <c r="G10" s="1"/>
       <c r="H10" s="6"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>11</v>
       </c>
@@ -888,7 +889,7 @@
       <c r="G11" s="5"/>
       <c r="H11" s="6"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>12</v>
       </c>
@@ -910,7 +911,7 @@
       <c r="G12" s="1"/>
       <c r="H12" s="6"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>13</v>
       </c>
@@ -932,7 +933,7 @@
       <c r="G13" s="5"/>
       <c r="H13" s="6"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>14</v>
       </c>
@@ -980,7 +981,7 @@
       </c>
       <c r="H15" s="6"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>16</v>
       </c>
@@ -1004,7 +1005,7 @@
       </c>
       <c r="H16" s="6"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>17</v>
       </c>
@@ -1028,7 +1029,7 @@
       </c>
       <c r="H17" s="6"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>18</v>
       </c>
@@ -1100,7 +1101,7 @@
       </c>
       <c r="H20" s="6"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>21</v>
       </c>
@@ -1122,7 +1123,7 @@
       <c r="G21" s="5"/>
       <c r="H21" s="6"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>22</v>
       </c>
@@ -1146,7 +1147,7 @@
       </c>
       <c r="H22" s="6"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>23</v>
       </c>
@@ -1219,7 +1220,13 @@
       <c r="H25" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H25" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:H25" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="Rahul"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Todo,WIP,Done"</formula1>

</xml_diff>

<commit_message>
Adavance Java PPT is in progress
Adavance Java PPT is in progress
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/DailyStatusTracker.xlsx
+++ b/Offline/BusinessManagement/DailyStatusTracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F0165E6-AAB3-4013-ADC1-59AE27DA44DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA1A3636-B3AE-4FE6-9514-18E2FE8F87CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="563" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="51">
   <si>
     <t>Item Description</t>
   </si>
@@ -184,9 +184,6 @@
   </si>
   <si>
     <t>Pending on Anttech business site defect closure</t>
-  </si>
-  <si>
-    <t>Done</t>
   </si>
   <si>
     <t>To be finished by 19-Feb</t>
@@ -607,7 +604,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
+      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -648,7 +645,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -694,7 +691,7 @@
       <c r="G3" s="5"/>
       <c r="H3" s="6"/>
     </row>
-    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -711,7 +708,7 @@
         <v>5</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="6"/>
@@ -740,7 +737,7 @@
       </c>
       <c r="H5" s="6"/>
     </row>
-    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -764,7 +761,7 @@
       </c>
       <c r="H6" s="6"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -854,7 +851,7 @@
       <c r="G10" s="5"/>
       <c r="H10" s="6"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -924,7 +921,7 @@
       </c>
       <c r="H13" s="6"/>
     </row>
-    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -996,7 +993,7 @@
       </c>
       <c r="H16" s="6"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -1018,7 +1015,7 @@
       <c r="G17" s="5"/>
       <c r="H17" s="6"/>
     </row>
-    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -1038,11 +1035,11 @@
         <v>6</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H18" s="6"/>
     </row>
-    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -1136,7 +1133,7 @@
       </c>
       <c r="H22" s="6"/>
     </row>
-    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -1164,7 +1161,7 @@
   <autoFilter ref="A1:H23" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <filterColumn colId="3">
       <filters>
-        <filter val="Debashish"/>
+        <filter val="Rahul"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>